<commit_message>
add filters and graphs
</commit_message>
<xml_diff>
--- a/Laufzeiten.xlsx
+++ b/Laufzeiten.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tuejc6\PycharmProjects\Streamlit_dash\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{527CF416-E559-47D9-8B45-36CE85B2A2A9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78C5218F-7A10-4F01-AFDB-867E67440DF2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14940" windowHeight="9840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="dd\.mm\.yyyy"/>
-    <numFmt numFmtId="166" formatCode="[h]:mm:ss;@"/>
+    <numFmt numFmtId="165" formatCode="[h]:mm:ss;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -82,7 +82,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
@@ -93,7 +93,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
@@ -103,6 +103,7 @@
     <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -321,10 +322,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -371,11 +372,11 @@
       </c>
       <c r="F2" s="4">
         <f>SUM(B:B)</f>
-        <v>121.60999999999997</v>
+        <v>127.80999999999997</v>
       </c>
       <c r="G2" s="13">
         <f>SUM(C:C)</f>
-        <v>0.49322916666666677</v>
+        <v>0.51822916666666674</v>
       </c>
       <c r="H2" s="6"/>
     </row>
@@ -390,7 +391,7 @@
         <v>2.5694444444444447E-2</v>
       </c>
       <c r="D3" s="11">
-        <f t="shared" ref="D3:D20" si="0">C3/B3</f>
+        <f t="shared" ref="D3:D21" si="0">C3/B3</f>
         <v>4.1309396212933199E-3</v>
       </c>
       <c r="H3" s="6"/>
@@ -546,7 +547,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
-        <v>48616</v>
+        <v>44963</v>
       </c>
       <c r="B13" s="1">
         <v>7.57</v>
@@ -672,6 +673,21 @@
         <v>4.0135902031063321E-3</v>
       </c>
       <c r="H20" s="6"/>
+    </row>
+    <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="14">
+        <v>44974</v>
+      </c>
+      <c r="B21" s="1">
+        <v>6.2</v>
+      </c>
+      <c r="C21" s="9">
+        <v>2.4999999999999998E-2</v>
+      </c>
+      <c r="D21" s="12">
+        <f t="shared" si="0"/>
+        <v>4.0322580645161289E-3</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D2:D20">

</xml_diff>